<commit_message>
Additional actions, js based string reversal added
</commit_message>
<xml_diff>
--- a/private/spreadsheet-template.xlsx
+++ b/private/spreadsheet-template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\codex-blackboard\codex-blackboard\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7590" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="9330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t/>
   </si>
@@ -92,9 +92,6 @@
     <t>Reverse a string</t>
   </si>
   <si>
-    <t>requires installing an App Script in this doc. Go to Insert-&gt;Script… and search for "string.reverse". Click install, and this should work correctly.</t>
-  </si>
-  <si>
     <t>The formulas in the Formula Cell column perform the named data transform on the cell directly to their left. To use, just copy/paste the contents as you need them.</t>
   </si>
   <si>
@@ -170,21 +167,12 @@
     <t>Strings</t>
   </si>
   <si>
-    <t>Consider chaining with binary to decimal</t>
-  </si>
-  <si>
     <t>Take character at Position</t>
   </si>
   <si>
     <t>Puzzle Text</t>
   </si>
   <si>
-    <t>Case insensitive. If you have a single shift value for multiple columns, change "C18" to "$C$18" (or wherever your index is) to have it stay static during copy/paste, or change it to a number</t>
-  </si>
-  <si>
-    <t>Case insensitive. If you have a single shift value for multiple columns, change "C19" to "$C$19" (or wherever your index is) to have it stay static during copy/paste, or change it to a number</t>
-  </si>
-  <si>
     <t>Remove Punctuation</t>
   </si>
   <si>
@@ -192,6 +180,50 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Deimal to Binary</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>ASCII letter to Number</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Take First Character</t>
+  </si>
+  <si>
+    <t>Decimal to Hexidecimal</t>
+  </si>
+  <si>
+    <t>Decimal to Octal</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Consider chaining with binary/decimal conversion</t>
+  </si>
+  <si>
+    <t>Case insensitive. If you have a single shift value for multiple columns, change "C22" to "$C$22" (or wherever your index is) to have it stay static during copy/paste, or change it to a number</t>
+  </si>
+  <si>
+    <t>Case insensitive. If you have a single shift value for multiple columns, change "C23" to "$C$23" (or wherever your index is) to have it stay static during copy/paste, or change it to a number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case insensitive. </t>
+  </si>
+  <si>
+    <t>function reverse(s){
+    return s.split("""").reverse().join("""");
+}</t>
+  </si>
+  <si>
+    <t>requires installing an App Script in this doc. Go to Insert-&gt;Script… and search for "string.reverse". Click install, and this should work correctly. Not guaranteed to work on non-English strings.</t>
   </si>
 </sst>
 </file>
@@ -250,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -298,6 +330,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1568,17 +1603,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="8" customWidth="1"/>
     <col min="6" max="6" width="85.7109375" customWidth="1"/>
@@ -1586,22 +1621,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
-      <c r="B1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1615,7 +1650,7 @@
     </row>
     <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -1648,11 +1683,11 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="11" t="str">
         <f>CHAR(MOD(D5,7)+64)</f>
@@ -1662,11 +1697,11 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="11" t="str">
         <f>CHAR(MOD(D6,10)+64)</f>
@@ -1676,11 +1711,11 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="11" t="str">
         <f>CHAR(MOD(D7,26)+64)</f>
@@ -1690,11 +1725,11 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="11" t="str">
         <f>CHAR(MOD(D8,100)+64)</f>
@@ -1702,232 +1737,301 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="11">
+        <f>CODE(D9)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="12" t="str">
-        <f>CHAR(D9)</f>
-        <v>M</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12" t="str">
+        <f>CHAR(D10)</f>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="11" t="str">
-        <f>CHAR(HEX2DEC(D10))</f>
+      <c r="E11" s="11" t="str">
+        <f>CHAR(HEX2DEC(D11))</f>
         <v>M</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="11" t="str">
-        <f>CHAR(HEX2DEC(D11)+64)</f>
-        <v>Z</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" s="11" t="str">
-        <f>CHAR(OCT2DEC(D12))</f>
-        <v>R</v>
+        <f>CHAR(HEX2DEC(D12)+64)</f>
+        <v>Z</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="11" t="str">
+        <f>CHAR(OCT2DEC(D13))</f>
+        <v>R</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="11" t="str">
+        <f>CHAR(OCT2DEC(D14)+64)</f>
+        <v>Q</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="11" t="str">
-        <f>CHAR(OCT2DEC(D13)+64)</f>
-        <v>Q</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="12">
-        <f>HEX2DEC(D14)</f>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3"/>
+      <c r="B15" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="13"/>
       <c r="D15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="12">
-        <f>OCT2DEC(D15)</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11" t="str">
+        <f>DEC2HEX(D15)</f>
+        <v>4D</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="6" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E16" s="12">
-        <f>BIN2DEC(D16)</f>
-        <v>107</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>19</v>
+        <f>HEX2DEC(D16)</f>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>17</v>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="E17" s="11" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(D17,0,2),1,0),2,1)</f>
-        <v>01101001</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+        <f>DEC2OCT(D17)</f>
         <v>47</v>
       </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18">
-        <v>-2</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="10" t="str">
-        <f>CHAR(MOD(CODE(UPPER(D18))-65+C18,26)+65 )</f>
-        <v>Y</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B19" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E18" s="12">
+        <f>OCT2DEC(D18)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="13"/>
       <c r="D19" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E19" s="12" t="str">
-        <f>UPPER(MID(D19,C19,1))</f>
-        <v>Z</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
+        <f>DEC2BIN(D19)</f>
+        <v>1000011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E20" s="12">
-        <f>IF(UPPER(D20)="BLACK",0,IF(UPPER(D20)="BROWN",1,IF(UPPER(D20)="TAN",1,IF(UPPER(D20)="RED",2,IF(UPPER(D20)="ORANGE",3,IF(UPPER(D20)="YELLOW",4,IF(UPPER(D20)="GREEN",5,IF(UPPER(D20)="BLUE",6,IF(UPPER(D20)="VIOLET",7,IF(UPPER(D20)="PURPLE",7,IF(UPPER(D20)="GREY",8,IF(UPPER(D20)="GRAY",8,IF(UPPER(D20)="WHITE",9,"Invalid Color")))))))))))))</f>
-        <v>1</v>
+        <f>BIN2DEC(D20)</f>
+        <v>107</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="11" t="e">
-        <f ca="1">reverse(D21)</f>
-        <v>#NAME?</v>
+        <v>17</v>
+      </c>
+      <c r="E21" s="11" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(D21,0,2),1,0),2,1)</f>
+        <v>01101001</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>-2</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="11" t="str">
-        <f>CHAR(ABS((CODE(UPPER(D22))-64)-26)+65)</f>
+        <v>37</v>
+      </c>
+      <c r="E22" s="10" t="str">
+        <f>CHAR(MOD(CODE(UPPER(D22))-65+C22,26)+65 )</f>
         <v>Y</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="14" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(D23,"'",""),"…","")," ",""),".",""),"!",""),"?","")</f>
+        <v>49</v>
+      </c>
+      <c r="E23" s="12" t="str">
+        <f>UPPER(MID(D23,C23,1))</f>
+        <v>Z</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="12" t="str">
+        <f>UPPER(LEFT(D24,1))</f>
+        <v>P</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="12">
+        <f>IF(UPPER(D25)="BLACK",0,IF(UPPER(D25)="BROWN",1,IF(UPPER(D25)="TAN",1,IF(UPPER(D25)="RED",2,IF(UPPER(D25)="ORANGE",3,IF(UPPER(D25)="YELLOW",4,IF(UPPER(D25)="GREEN",5,IF(UPPER(D25)="BLUE",6,IF(UPPER(D25)="VIOLET",7,IF(UPPER(D25)="PURPLE",7,IF(UPPER(D25)="GREY",8,IF(UPPER(D25)="GRAY",8,IF(UPPER(D25)="WHITE",9,"Invalid Color")))))))))))))</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="11" t="str">
+        <f>CHAR(ABS((CODE(UPPER(D26))-64)-26)+65)</f>
+        <v>Y</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="11" t="e">
+        <f ca="1">reverse(D27)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="14" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(D28,"'",""),"…","")," ",""),".",""),"!",""),"?","")</f>
         <v>PuzzleText</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E24" s="15"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>